<commit_message>
adjustments to the excel sheet, and a data collection code for the arduino
</commit_message>
<xml_diff>
--- a/Product list.xlsx
+++ b/Product list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aankit\Desktop\Homework\Engineering code Screenshots\ENGR122\Design project\ENGR122-Design-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF5AD7C-4229-4543-9E67-5691FBFF9C02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6E0C8F-220C-40A1-ABDE-661279819842}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A9A8D031-D6AF-4A9F-A939-166BDEB0D294}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A9A8D031-D6AF-4A9F-A939-166BDEB0D294}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>amt</t>
   </si>
@@ -84,6 +84,21 @@
   </si>
   <si>
     <t>https://www.walmart.com/search/?query=transistors</t>
+  </si>
+  <si>
+    <t>ordered?</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>No need</t>
+  </si>
+  <si>
+    <t>no need</t>
   </si>
 </sst>
 </file>
@@ -107,7 +122,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -116,18 +131,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -136,18 +157,29 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -155,11 +187,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -475,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B1A7ED8-752F-4670-A412-C3C1A4EB2D81}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,92 +521,122 @@
     <col min="3" max="3" width="117.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="D3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>1</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <v>4</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>16</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -582,5 +646,6 @@
     <hyperlink ref="C8" r:id="rId3" xr:uid="{71A13330-CB1C-49D8-9B6D-03E8C63B78DB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>